<commit_message>
grog, new models, frontend loading icon
</commit_message>
<xml_diff>
--- a/labeled_036.xlsx
+++ b/labeled_036.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RaChr\Desktop\Skole\Bachelor\Ai-Bachelor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF2DE7B-2A57-4A88-818F-C0124EF1E943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06F7BFC-52C3-4AD0-A17D-B42896370713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27780" yWindow="0" windowWidth="23925" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2658,8 +2658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I705"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B202" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E237" sqref="E237"/>
+    <sheetView tabSelected="1" topLeftCell="B131" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H161" sqref="H161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5063,6 +5063,9 @@
       <c r="E96" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="H96" t="b">
+        <v>0</v>
+      </c>
       <c r="I96" s="1" t="s">
         <v>97</v>
       </c>
@@ -5083,6 +5086,9 @@
       <c r="E97" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="H97" t="b">
+        <v>0</v>
+      </c>
       <c r="I97" s="1" t="s">
         <v>98</v>
       </c>
@@ -5103,6 +5109,9 @@
       <c r="E98" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="H98" t="b">
+        <v>0</v>
+      </c>
       <c r="I98" s="1" t="s">
         <v>99</v>
       </c>
@@ -5123,6 +5132,9 @@
       <c r="E99" s="1" t="s">
         <v>100</v>
       </c>
+      <c r="H99" t="b">
+        <v>0</v>
+      </c>
       <c r="I99" s="1" t="s">
         <v>100</v>
       </c>
@@ -5288,6 +5300,9 @@
       <c r="E105" s="1" t="s">
         <v>106</v>
       </c>
+      <c r="H105" t="b">
+        <v>0</v>
+      </c>
       <c r="I105" s="1" t="s">
         <v>106</v>
       </c>
@@ -5308,6 +5323,9 @@
       <c r="E106" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="H106" t="b">
+        <v>0</v>
+      </c>
       <c r="I106" s="1" t="s">
         <v>107</v>
       </c>
@@ -5502,6 +5520,9 @@
       <c r="E113" s="1" t="s">
         <v>114</v>
       </c>
+      <c r="H113" t="b">
+        <v>0</v>
+      </c>
       <c r="I113" s="1" t="s">
         <v>114</v>
       </c>
@@ -5522,6 +5543,9 @@
       <c r="E114" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="H114" t="b">
+        <v>0</v>
+      </c>
       <c r="I114" s="1" t="s">
         <v>115</v>
       </c>
@@ -5542,6 +5566,9 @@
       <c r="E115" s="1" t="s">
         <v>116</v>
       </c>
+      <c r="H115" t="b">
+        <v>0</v>
+      </c>
       <c r="I115" s="1" t="s">
         <v>116</v>
       </c>
@@ -5562,6 +5589,9 @@
       <c r="E116" s="1" t="s">
         <v>117</v>
       </c>
+      <c r="H116" t="b">
+        <v>0</v>
+      </c>
       <c r="I116" s="1" t="s">
         <v>117</v>
       </c>
@@ -5582,6 +5612,9 @@
       <c r="E117" s="1" t="s">
         <v>118</v>
       </c>
+      <c r="H117" t="b">
+        <v>0</v>
+      </c>
       <c r="I117" s="1" t="s">
         <v>118</v>
       </c>
@@ -5602,6 +5635,9 @@
       <c r="E118" s="1" t="s">
         <v>119</v>
       </c>
+      <c r="H118" t="b">
+        <v>0</v>
+      </c>
       <c r="I118" s="1" t="s">
         <v>119</v>
       </c>
@@ -5622,6 +5658,9 @@
       <c r="E119" s="1" t="s">
         <v>120</v>
       </c>
+      <c r="H119" t="b">
+        <v>0</v>
+      </c>
       <c r="I119" s="1" t="s">
         <v>120</v>
       </c>
@@ -5642,6 +5681,9 @@
       <c r="E120" s="1" t="s">
         <v>121</v>
       </c>
+      <c r="H120" t="b">
+        <v>0</v>
+      </c>
       <c r="I120" s="1" t="s">
         <v>121</v>
       </c>
@@ -5662,6 +5704,9 @@
       <c r="E121" s="1" t="s">
         <v>122</v>
       </c>
+      <c r="H121" t="b">
+        <v>0</v>
+      </c>
       <c r="I121" s="1" t="s">
         <v>122</v>
       </c>
@@ -5682,6 +5727,9 @@
       <c r="E122" s="1" t="s">
         <v>123</v>
       </c>
+      <c r="H122" t="b">
+        <v>0</v>
+      </c>
       <c r="I122" s="1" t="s">
         <v>123</v>
       </c>
@@ -5702,6 +5750,9 @@
       <c r="E123" s="1" t="s">
         <v>124</v>
       </c>
+      <c r="H123" t="b">
+        <v>0</v>
+      </c>
       <c r="I123" s="1" t="s">
         <v>124</v>
       </c>
@@ -5722,6 +5773,9 @@
       <c r="E124" s="1" t="s">
         <v>125</v>
       </c>
+      <c r="H124" t="b">
+        <v>0</v>
+      </c>
       <c r="I124" s="1" t="s">
         <v>125</v>
       </c>
@@ -5965,6 +6019,9 @@
       <c r="E133" s="1" t="s">
         <v>134</v>
       </c>
+      <c r="H133" t="b">
+        <v>0</v>
+      </c>
       <c r="I133" s="1" t="s">
         <v>134</v>
       </c>
@@ -5985,6 +6042,9 @@
       <c r="E134" s="1" t="s">
         <v>135</v>
       </c>
+      <c r="H134" t="b">
+        <v>0</v>
+      </c>
       <c r="I134" s="1" t="s">
         <v>135</v>
       </c>
@@ -6005,6 +6065,9 @@
       <c r="E135" s="1" t="s">
         <v>136</v>
       </c>
+      <c r="H135" t="b">
+        <v>0</v>
+      </c>
       <c r="I135" s="1" t="s">
         <v>136</v>
       </c>
@@ -6025,6 +6088,9 @@
       <c r="E136" s="1" t="s">
         <v>137</v>
       </c>
+      <c r="H136" t="b">
+        <v>0</v>
+      </c>
       <c r="I136" s="1" t="s">
         <v>137</v>
       </c>
@@ -6045,6 +6111,9 @@
       <c r="E137" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="H137" t="b">
+        <v>0</v>
+      </c>
       <c r="I137" s="1" t="s">
         <v>59</v>
       </c>
@@ -6065,6 +6134,9 @@
       <c r="E138" s="1" t="s">
         <v>138</v>
       </c>
+      <c r="H138" t="b">
+        <v>0</v>
+      </c>
       <c r="I138" s="1" t="s">
         <v>138</v>
       </c>
@@ -6085,6 +6157,9 @@
       <c r="E139" s="1" t="s">
         <v>139</v>
       </c>
+      <c r="H139" t="b">
+        <v>0</v>
+      </c>
       <c r="I139" s="1" t="s">
         <v>139</v>
       </c>
@@ -6105,6 +6180,9 @@
       <c r="E140" s="1" t="s">
         <v>140</v>
       </c>
+      <c r="H140" t="b">
+        <v>0</v>
+      </c>
       <c r="I140" s="1" t="s">
         <v>140</v>
       </c>
@@ -6125,6 +6203,9 @@
       <c r="E141" s="1" t="s">
         <v>141</v>
       </c>
+      <c r="H141" t="b">
+        <v>0</v>
+      </c>
       <c r="I141" s="1" t="s">
         <v>141</v>
       </c>
@@ -6145,6 +6226,9 @@
       <c r="E142" s="1" t="s">
         <v>142</v>
       </c>
+      <c r="H142" t="b">
+        <v>0</v>
+      </c>
       <c r="I142" s="1" t="s">
         <v>142</v>
       </c>
@@ -6165,6 +6249,9 @@
       <c r="E143" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="H143" t="b">
+        <v>0</v>
+      </c>
       <c r="I143" s="1" t="s">
         <v>143</v>
       </c>
@@ -6185,6 +6272,9 @@
       <c r="E144" s="1" t="s">
         <v>144</v>
       </c>
+      <c r="H144" t="b">
+        <v>0</v>
+      </c>
       <c r="I144" s="1" t="s">
         <v>144</v>
       </c>
@@ -6205,6 +6295,9 @@
       <c r="E145" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="H145" t="b">
+        <v>0</v>
+      </c>
       <c r="I145" s="1" t="s">
         <v>145</v>
       </c>
@@ -6225,6 +6318,9 @@
       <c r="E146" s="1" t="s">
         <v>146</v>
       </c>
+      <c r="H146" t="b">
+        <v>0</v>
+      </c>
       <c r="I146" s="1" t="s">
         <v>146</v>
       </c>
@@ -6245,6 +6341,9 @@
       <c r="E147" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="H147" t="b">
+        <v>0</v>
+      </c>
       <c r="I147" s="1" t="s">
         <v>147</v>
       </c>
@@ -6265,6 +6364,9 @@
       <c r="E148" s="1" t="s">
         <v>148</v>
       </c>
+      <c r="H148" t="b">
+        <v>0</v>
+      </c>
       <c r="I148" s="1" t="s">
         <v>148</v>
       </c>
@@ -6285,6 +6387,9 @@
       <c r="E149" s="1" t="s">
         <v>149</v>
       </c>
+      <c r="H149" t="b">
+        <v>0</v>
+      </c>
       <c r="I149" s="1" t="s">
         <v>149</v>
       </c>
@@ -6305,6 +6410,9 @@
       <c r="E150" s="1" t="s">
         <v>150</v>
       </c>
+      <c r="H150" t="b">
+        <v>0</v>
+      </c>
       <c r="I150" s="1" t="s">
         <v>150</v>
       </c>
@@ -6325,6 +6433,9 @@
       <c r="E151" s="1" t="s">
         <v>151</v>
       </c>
+      <c r="H151" t="b">
+        <v>0</v>
+      </c>
       <c r="I151" s="1" t="s">
         <v>151</v>
       </c>
@@ -6345,6 +6456,9 @@
       <c r="E152" s="1" t="s">
         <v>152</v>
       </c>
+      <c r="H152" t="b">
+        <v>0</v>
+      </c>
       <c r="I152" s="1" t="s">
         <v>152</v>
       </c>
@@ -6394,6 +6508,9 @@
       <c r="E154" s="1" t="s">
         <v>154</v>
       </c>
+      <c r="H154" t="b">
+        <v>0</v>
+      </c>
       <c r="I154" s="1" t="s">
         <v>154</v>
       </c>
@@ -6413,6 +6530,9 @@
       </c>
       <c r="E155" s="1" t="s">
         <v>155</v>
+      </c>
+      <c r="H155" t="b">
+        <v>0</v>
       </c>
       <c r="I155" s="1" t="s">
         <v>155</v>
@@ -20440,15 +20560,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008BA4CACCB295284C9543D57370035B11" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8d0b1e45dff6aff44695dc5f2bd716cb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="017d1f16-6d54-4c23-a67a-b7f84f6bb8a0" xmlns:ns3="889e7f7e-cb63-460b-b277-b78afa20c8c9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b4f609581bb41a1140eef53502fe361e" ns2:_="" ns3:_="">
     <xsd:import namespace="017d1f16-6d54-4c23-a67a-b7f84f6bb8a0"/>
@@ -20671,15 +20782,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{039AC793-FA86-46F9-BE66-8DD75116057E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA829C32-D33B-4DE9-9328-4A862E372DF4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20696,4 +20808,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{039AC793-FA86-46F9-BE66-8DD75116057E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>